<commit_message>
routeo sallen key terminado
</commit_message>
<xml_diff>
--- a/Diseño/polez_zeros_legendre.xlsx
+++ b/Diseño/polez_zeros_legendre.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joaco\Desktop\repos\TC\TP7\Diseño\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6EB2731-9860-4523-A1E9-B1632F8542B4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27C9855B-8D57-493B-B4D0-8AA1905665D9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-10092" yWindow="5316" windowWidth="17280" windowHeight="8964" activeTab="3" xr2:uid="{832EFF2D-5292-4B1D-BA49-1F4645D26A27}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{832EFF2D-5292-4B1D-BA49-1F4645D26A27}"/>
   </bookViews>
   <sheets>
     <sheet name="Conf. 1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="7">
   <si>
     <t>Pole Q</t>
   </si>
@@ -1377,7 +1377,7 @@
   <dimension ref="A2:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>